<commit_message>
Enhance scraping functionality with real-time updates and search interruption support
</commit_message>
<xml_diff>
--- a/data/viviendas.xlsx
+++ b/data/viviendas.xlsx
@@ -587,7 +587,11 @@
       <c r="I2" t="n">
         <v>0</v>
       </c>
-      <c r="J2" t="inlineStr"/>
+      <c r="J2" t="inlineStr">
+        <is>
+          <t>648 74 65 62</t>
+        </is>
+      </c>
       <c r="K2" t="inlineStr">
         <is>
           <t>ParticularJessica</t>
@@ -605,12 +609,12 @@
       </c>
       <c r="N2" t="inlineStr">
         <is>
-          <t>2025-09-17 08:15:58</t>
+          <t>2025-09-17 13:14:08</t>
         </is>
       </c>
       <c r="O2" t="inlineStr">
         <is>
-          <t>2025-09-17 10:06:08</t>
+          <t>2025-09-17 13:14:08</t>
         </is>
       </c>
       <c r="P2" t="inlineStr">
@@ -658,7 +662,11 @@
       <c r="I3" t="n">
         <v>0</v>
       </c>
-      <c r="J3" t="inlineStr"/>
+      <c r="J3" t="inlineStr">
+        <is>
+          <t>635 57 00 94</t>
+        </is>
+      </c>
       <c r="K3" t="inlineStr">
         <is>
           <t>ParticularJoan Luis Morales</t>
@@ -676,12 +684,12 @@
       </c>
       <c r="N3" t="inlineStr">
         <is>
-          <t>2025-09-17 08:15:58</t>
+          <t>2025-09-17 13:25:58</t>
         </is>
       </c>
       <c r="O3" t="inlineStr">
         <is>
-          <t>2025-09-17 10:06:08</t>
+          <t>2025-09-17 13:25:58</t>
         </is>
       </c>
       <c r="P3" t="inlineStr">
@@ -729,7 +737,11 @@
       <c r="I4" t="n">
         <v>0</v>
       </c>
-      <c r="J4" t="inlineStr"/>
+      <c r="J4" t="inlineStr">
+        <is>
+          <t>630 23 45 85</t>
+        </is>
+      </c>
       <c r="K4" t="inlineStr">
         <is>
           <t>ParticularGuifré Badosa</t>
@@ -747,12 +759,12 @@
       </c>
       <c r="N4" t="inlineStr">
         <is>
-          <t>2025-09-17 08:15:58</t>
+          <t>2025-09-17 13:25:58</t>
         </is>
       </c>
       <c r="O4" t="inlineStr">
         <is>
-          <t>2025-09-17 10:06:08</t>
+          <t>2025-09-17 13:25:58</t>
         </is>
       </c>
       <c r="P4" t="inlineStr">
@@ -800,7 +812,11 @@
       <c r="I5" t="n">
         <v>0</v>
       </c>
-      <c r="J5" t="inlineStr"/>
+      <c r="J5" t="inlineStr">
+        <is>
+          <t>644 49 22 12</t>
+        </is>
+      </c>
       <c r="K5" t="inlineStr">
         <is>
           <t>ParticularTeo</t>
@@ -818,12 +834,12 @@
       </c>
       <c r="N5" t="inlineStr">
         <is>
-          <t>2025-09-17 08:15:58</t>
+          <t>2025-09-17 13:25:58</t>
         </is>
       </c>
       <c r="O5" t="inlineStr">
         <is>
-          <t>2025-09-17 10:06:08</t>
+          <t>2025-09-17 13:25:58</t>
         </is>
       </c>
       <c r="P5" t="inlineStr">
@@ -871,7 +887,11 @@
       <c r="I6" t="n">
         <v>0</v>
       </c>
-      <c r="J6" t="inlineStr"/>
+      <c r="J6" t="inlineStr">
+        <is>
+          <t>644 49 22 12</t>
+        </is>
+      </c>
       <c r="K6" t="inlineStr">
         <is>
           <t>ParticularTeo</t>
@@ -889,12 +909,12 @@
       </c>
       <c r="N6" t="inlineStr">
         <is>
-          <t>2025-09-17 08:15:58</t>
+          <t>2025-09-17 13:25:58</t>
         </is>
       </c>
       <c r="O6" t="inlineStr">
         <is>
-          <t>2025-09-17 10:06:08</t>
+          <t>2025-09-17 13:25:58</t>
         </is>
       </c>
       <c r="P6" t="inlineStr">

</xml_diff>